<commit_message>
added presentation and excel evaluation
</commit_message>
<xml_diff>
--- a/questionnaire/shuffled/Daniel questionnaires.xlsx
+++ b/questionnaire/shuffled/Daniel questionnaires.xlsx
@@ -5,23 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Desktop\COV\cov-generative-ai\questionnaire\shuffled\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\cov-generative-ai\questionnaire\shuffled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF167852-8507-4C3C-8EDC-468AFDF7674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C52BC-4055-4214-B682-A3256B595998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Person 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Person 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Person 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Person 4" sheetId="5" r:id="rId4"/>
-    <sheet name="Person 5" sheetId="6" r:id="rId5"/>
-    <sheet name="Person x" sheetId="7" r:id="rId6"/>
-    <sheet name="Person 7" sheetId="8" r:id="rId7"/>
-    <sheet name="Person 8" sheetId="9" r:id="rId8"/>
+    <sheet name="Auswertung" sheetId="10" r:id="rId1"/>
+    <sheet name="Person 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Person 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Person 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Person 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Person 5" sheetId="6" r:id="rId6"/>
+    <sheet name="Person x" sheetId="7" r:id="rId7"/>
+    <sheet name="Person 7" sheetId="8" r:id="rId8"/>
+    <sheet name="Person 8" sheetId="9" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="30">
   <si>
     <t>Bild-Nummer</t>
   </si>
@@ -125,6 +129,15 @@
   <si>
     <t>Farbe, Wenn hohe Sättigung, Symmetrie, fette Käseschicht, einheitlicher Teig, Hintergrund, Daumen eher echt, imperfections -&gt; eher echt</t>
   </si>
+  <si>
+    <t>confusion matrix</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
 </sst>
 </file>
 
@@ -176,6 +189,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Person 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="7">
+          <cell r="B7">
+            <v>13</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,20 +475,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC3BAB5-A68E-491B-925B-DAF49D0C70B4}">
+  <dimension ref="F5:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="6" width="14.61328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="6:15" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="6:15" x14ac:dyDescent="0.4">
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:15" x14ac:dyDescent="0.4">
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <f>('Person 1'!B7+'Person 2'!B7+'Person 3'!B7+'Person 4'!B7+'Person 5'!B7+'Person x'!B7+'Person 7'!B7+'Person 8'!B7+'[1]Person 1'!$B$7)/9</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="J7">
+        <f>('Person 1'!C7+'Person 2'!C7+'Person 3'!C7+'Person 4'!C7+'Person 5'!C7+'Person x'!C7+'Person 7'!C7+'Person 8'!C7+'[1]Person 1'!$B$7)/9</f>
+        <v>7.1111111111111107</v>
+      </c>
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <f>_xlfn.STDEV.S('Person 1'!B7,'Person 2'!B7,'Person 3'!B7,'Person 4'!B7,'Person 5'!B7,'Person x'!B7,'Person 7'!B7,'Person 8'!B7,'[1]Person 1'!$B$7)</f>
+        <v>3.905124837953327</v>
+      </c>
+      <c r="O7">
+        <f>_xlfn.STDEV.S('Person 1'!C7,'Person 2'!C7,'Person 3'!C7,'Person 4'!C7,'Person 5'!C7,'Person x'!C7,'Person 7'!C7,'Person 8'!C7,'[1]Person 1'!$B$7)</f>
+        <v>4.9860917672171974</v>
+      </c>
+    </row>
+    <row r="8" spans="6:15" x14ac:dyDescent="0.4">
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f>('Person 1'!B8+'Person 2'!B8+'Person 3'!B8+'Person 4'!B8+'Person 5'!B8+'Person x'!B8+'Person 7'!B8+'Person 8'!B8+'[1]Person 1'!$B$7)/9</f>
+        <v>5.8888888888888893</v>
+      </c>
+      <c r="J8">
+        <f>('Person 1'!C8+'Person 2'!C8+'Person 3'!C8+'Person 4'!C8+'Person 5'!C8+'Person x'!C8+'Person 7'!C8+'Person 8'!C8+'[1]Person 1'!$B$7)/9</f>
+        <v>9.1111111111111107</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <f>_xlfn.STDEV.S('Person 1'!B8,'Person 2'!B8,'Person 3'!B8,'Person 4'!B8,'Person 5'!B8,'Person x'!B8,'Person 7'!B8,'Person 8'!B8,'[1]Person 1'!$B$7)</f>
+        <v>4.6218082079540164</v>
+      </c>
+      <c r="O8">
+        <f>_xlfn.STDEV.S('Person 1'!C8,'Person 2'!C8,'Person 3'!C8,'Person 4'!C8,'Person 5'!C8,'Person x'!C8,'Person 7'!C8,'Person 8'!C8,'[1]Person 1'!$B$7)</f>
+        <v>4.7022453265552953</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -643,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -738,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -746,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -759,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -772,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -782,7 +910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859B0D4B-007C-437A-9B12-376DE388A59D}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
@@ -790,13 +918,13 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +1019,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -986,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +1209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1115,32 +1243,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1150,7 +1278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83921-8BD0-487F-B188-ADB8B36C23DF}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
@@ -1158,13 +1286,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1387,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1354,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1449,7 +1577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1457,7 +1585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1483,27 +1611,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1513,7 +1641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC77678-2515-4B16-8EE9-B5D14F719BB0}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
@@ -1521,13 +1649,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1750,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1717,7 +1845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1812,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1833,7 +1961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1846,7 +1974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1856,7 +1984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C801AA7-5A7C-4043-A858-2657B0A59ED6}">
   <dimension ref="A1:AE14"/>
   <sheetViews>
@@ -1864,13 +1992,13 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1965,7 +2093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2155,7 +2283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2163,7 +2291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2176,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2189,22 +2317,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2214,7 +2342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AC0ABD-675A-43B8-ADAE-4892D49980D6}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
@@ -2222,13 +2350,13 @@
       <selection activeCell="E15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2323,7 +2451,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2418,7 +2546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2513,7 +2641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2521,7 +2649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2547,7 +2675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2557,7 +2685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C4A73-13F6-4C8A-BB04-B96FE9EA3418}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
@@ -2565,13 +2693,13 @@
       <selection activeCell="L26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2856,7 +2984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2864,7 +2992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2877,7 +3005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2890,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2900,21 +3028,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E5A7E-357C-4099-82CD-8DF45C0865CA}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3009,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3104,7 +3232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3199,7 +3327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -3207,7 +3335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3220,7 +3348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3233,7 +3361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>26</v>
       </c>

</xml_diff>